<commit_message>
Updated Bills and Receipts CRUD operations.
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -441,7 +441,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,22 +498,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -524,22 +524,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>1</v>

</xml_diff>

<commit_message>
Update Members and People CRUD
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -441,7 +441,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,6 +498,7 @@
         <v>1</v>
       </c>
       <c r="B3">
+        <f>IF(SUM(C3:H3)=6,1,IF(SUM(C3:H3)&gt;-6,0,-1))</f>
         <v>1</v>
       </c>
       <c r="C3">
@@ -524,6 +525,7 @@
         <v>2</v>
       </c>
       <c r="B4">
+        <f t="shared" ref="B4:B22" si="0">IF(SUM(C4:H4)=6,1,IF(SUM(C4:H4)&gt;-6,0,-1))</f>
         <v>1</v>
       </c>
       <c r="C4">
@@ -550,22 +552,23 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -576,22 +579,23 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -602,7 +606,8 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>-1</v>
       </c>
       <c r="C7">
         <v>-1</v>
@@ -628,7 +633,8 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>-1</v>
@@ -654,6 +660,7 @@
         <v>7</v>
       </c>
       <c r="B9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C9">
@@ -680,7 +687,8 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -706,6 +714,7 @@
         <v>15</v>
       </c>
       <c r="B11">
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="C11">
@@ -732,6 +741,7 @@
         <v>16</v>
       </c>
       <c r="B12">
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="C12">
@@ -758,6 +768,7 @@
         <v>17</v>
       </c>
       <c r="B13">
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="C13">
@@ -784,6 +795,7 @@
         <v>18</v>
       </c>
       <c r="B14">
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="C14">
@@ -810,6 +822,7 @@
         <v>19</v>
       </c>
       <c r="B15">
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="C15">
@@ -836,7 +849,8 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>-1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>-1</v>
@@ -862,7 +876,8 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>-1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -888,7 +903,8 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>-1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="C18">
         <v>-1</v>
@@ -914,7 +930,8 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>-1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="C19">
         <v>-1</v>
@@ -940,7 +957,8 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>-1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="C20">
         <v>-1</v>
@@ -966,7 +984,8 @@
         <v>25</v>
       </c>
       <c r="B21">
-        <v>-1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -992,6 +1011,7 @@
         <v>26</v>
       </c>
       <c r="B22">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C22">
@@ -1026,7 +1046,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:H15">
+  <conditionalFormatting sqref="B3:H3 C4:H15 B4:B22">
     <cfRule type="iconSet" priority="11">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
@@ -1035,7 +1055,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:H22">
+  <conditionalFormatting sqref="C16:H22">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>

</xml_diff>

<commit_message>
Update Balances and Login
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -129,12 +129,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -149,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -158,6 +170,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,7 +539,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B22" si="0">IF(SUM(C4:H4)=6,1,IF(SUM(C4:H4)&gt;-6,0,-1))</f>
+        <f t="shared" ref="B4:B24" si="0">IF(SUM(C4:H4)=6,1,IF(SUM(C4:H4)&gt;-6,0,-1))</f>
         <v>1</v>
       </c>
       <c r="C4">
@@ -603,11 +617,11 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>-1</v>
@@ -625,31 +639,31 @@
         <v>-1</v>
       </c>
       <c r="H7">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -657,7 +671,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
@@ -670,366 +684,366 @@
         <v>-1</v>
       </c>
       <c r="E9">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5">
+        <f>IF(SUM(C11:H11)=6,1,IF(SUM(C11:H11)&gt;-6,0,-1))</f>
+        <v>-1</v>
+      </c>
+      <c r="C11" s="5">
+        <v>-1</v>
+      </c>
+      <c r="D11" s="5">
+        <v>-1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F11" s="5">
+        <v>-1</v>
+      </c>
+      <c r="G11" s="5">
+        <v>-1</v>
+      </c>
+      <c r="H11" s="5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="C13" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>-1</v>
+      </c>
+      <c r="E13" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F13" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G13" s="4">
+        <v>-1</v>
+      </c>
+      <c r="H13" s="4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="4">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="C14" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D14" s="4">
+        <v>-1</v>
+      </c>
+      <c r="E14" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F14" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G14" s="4">
+        <v>-1</v>
+      </c>
+      <c r="H14" s="4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="4">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="C15" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D15" s="4">
+        <v>-1</v>
+      </c>
+      <c r="E15" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F15" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G15" s="4">
+        <v>-1</v>
+      </c>
+      <c r="H15" s="4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="4">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="C16" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D16" s="4">
+        <v>-1</v>
+      </c>
+      <c r="E16" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F16" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G16" s="4">
+        <v>-1</v>
+      </c>
+      <c r="H16" s="4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="4">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="C17" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D17" s="4">
+        <v>-1</v>
+      </c>
+      <c r="E17" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F17" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G17" s="4">
+        <v>-1</v>
+      </c>
+      <c r="H17" s="4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>-1</v>
-      </c>
-      <c r="E10">
-        <v>-1</v>
-      </c>
-      <c r="F10">
-        <v>-1</v>
-      </c>
-      <c r="G10">
-        <v>-1</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="C11">
-        <v>-1</v>
-      </c>
-      <c r="D11">
-        <v>-1</v>
-      </c>
-      <c r="E11">
-        <v>-1</v>
-      </c>
-      <c r="F11">
-        <v>-1</v>
-      </c>
-      <c r="G11">
-        <v>-1</v>
-      </c>
-      <c r="H11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="C12">
-        <v>-1</v>
-      </c>
-      <c r="D12">
-        <v>-1</v>
-      </c>
-      <c r="E12">
-        <v>-1</v>
-      </c>
-      <c r="F12">
-        <v>-1</v>
-      </c>
-      <c r="G12">
-        <v>-1</v>
-      </c>
-      <c r="H12">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="C13">
-        <v>-1</v>
-      </c>
-      <c r="D13">
-        <v>-1</v>
-      </c>
-      <c r="E13">
-        <v>-1</v>
-      </c>
-      <c r="F13">
-        <v>-1</v>
-      </c>
-      <c r="G13">
-        <v>-1</v>
-      </c>
-      <c r="H13">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="C14">
-        <v>-1</v>
-      </c>
-      <c r="D14">
-        <v>-1</v>
-      </c>
-      <c r="E14">
-        <v>-1</v>
-      </c>
-      <c r="F14">
-        <v>-1</v>
-      </c>
-      <c r="G14">
-        <v>-1</v>
-      </c>
-      <c r="H14">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="C15">
-        <v>-1</v>
-      </c>
-      <c r="D15">
-        <v>-1</v>
-      </c>
-      <c r="E15">
-        <v>-1</v>
-      </c>
-      <c r="F15">
-        <v>-1</v>
-      </c>
-      <c r="G15">
-        <v>-1</v>
-      </c>
-      <c r="H15">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16">
+      <c r="C18" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D18" s="4">
+        <v>-1</v>
+      </c>
+      <c r="E18" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F18" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G18" s="4">
+        <v>-1</v>
+      </c>
+      <c r="H18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C16">
-        <v>-1</v>
-      </c>
-      <c r="D16">
-        <v>-1</v>
-      </c>
-      <c r="E16">
-        <v>-1</v>
-      </c>
-      <c r="F16">
-        <v>-1</v>
-      </c>
-      <c r="G16">
-        <v>-1</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17">
+      <c r="C19" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D19" s="4">
+        <v>-1</v>
+      </c>
+      <c r="E19" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F19" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G19" s="4">
+        <v>-1</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C17">
-        <v>-1</v>
-      </c>
-      <c r="D17">
-        <v>-1</v>
-      </c>
-      <c r="E17">
-        <v>-1</v>
-      </c>
-      <c r="F17">
-        <v>-1</v>
-      </c>
-      <c r="G17">
-        <v>-1</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18">
+      <c r="C20" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D20" s="4">
+        <v>-1</v>
+      </c>
+      <c r="E20" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F20" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G20" s="4">
+        <v>-1</v>
+      </c>
+      <c r="H20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C18">
-        <v>-1</v>
-      </c>
-      <c r="D18">
-        <v>-1</v>
-      </c>
-      <c r="E18">
-        <v>-1</v>
-      </c>
-      <c r="F18">
-        <v>-1</v>
-      </c>
-      <c r="G18">
-        <v>-1</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19">
+      <c r="C21" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D21" s="4">
+        <v>-1</v>
+      </c>
+      <c r="E21" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F21" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G21" s="4">
+        <v>-1</v>
+      </c>
+      <c r="H21" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C19">
-        <v>-1</v>
-      </c>
-      <c r="D19">
-        <v>-1</v>
-      </c>
-      <c r="E19">
-        <v>-1</v>
-      </c>
-      <c r="F19">
-        <v>-1</v>
-      </c>
-      <c r="G19">
-        <v>-1</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20">
+      <c r="C22" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D22" s="4">
+        <v>-1</v>
+      </c>
+      <c r="E22" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F22" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G22" s="4">
+        <v>-1</v>
+      </c>
+      <c r="H22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C20">
-        <v>-1</v>
-      </c>
-      <c r="D20">
-        <v>-1</v>
-      </c>
-      <c r="E20">
-        <v>-1</v>
-      </c>
-      <c r="F20">
-        <v>-1</v>
-      </c>
-      <c r="G20">
-        <v>-1</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21">
+      <c r="C23" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D23" s="4">
+        <v>-1</v>
+      </c>
+      <c r="E23" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F23" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G23" s="4">
+        <v>-1</v>
+      </c>
+      <c r="H23" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C21">
-        <v>-1</v>
-      </c>
-      <c r="D21">
-        <v>-1</v>
-      </c>
-      <c r="E21">
-        <v>-1</v>
-      </c>
-      <c r="F21">
-        <v>-1</v>
-      </c>
-      <c r="G21">
-        <v>-1</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>-1</v>
-      </c>
-      <c r="D22">
-        <v>-1</v>
-      </c>
-      <c r="E22">
-        <v>-1</v>
-      </c>
-      <c r="F22">
-        <v>-1</v>
-      </c>
-      <c r="G22">
-        <v>-1</v>
-      </c>
-      <c r="H22">
+      <c r="C24" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D24" s="4">
+        <v>-1</v>
+      </c>
+      <c r="E24" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F24" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G24" s="4">
+        <v>-1</v>
+      </c>
+      <c r="H24" s="4">
         <v>1</v>
       </c>
     </row>
@@ -1037,7 +1051,7 @@
   <mergeCells count="1">
     <mergeCell ref="C1:F1"/>
   </mergeCells>
-  <conditionalFormatting sqref="N8">
+  <conditionalFormatting sqref="N7">
     <cfRule type="iconSet" priority="7">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
@@ -1046,7 +1060,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:H3 C4:H15 B4:B22">
+  <conditionalFormatting sqref="B3:H11 B12:B24 C12:H17">
     <cfRule type="iconSet" priority="11">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
@@ -1055,7 +1069,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C16:H22">
+  <conditionalFormatting sqref="C18:H24">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
@@ -1083,7 +1097,7 @@
               </x14:cfvo>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>L18:N18</xm:sqref>
+          <xm:sqref>L20:N20</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>